<commit_message>
get the 30 most popular currencies
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,7 +447,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="9.6" customWidth="1" min="1" max="1"/>
-    <col width="7.199999999999999" customWidth="1" min="2" max="2"/>
+    <col width="9.6" customWidth="1" min="2" max="2"/>
     <col width="13.2" customWidth="1" min="3" max="3"/>
     <col width="20.4" customWidth="1" min="4" max="4"/>
     <col width="16.8" customWidth="1" min="5" max="5"/>
@@ -487,13 +487,13 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>21092.95</v>
+        <v>21084.02</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>406347673723.6823</v>
+        <v>406175601662.3179</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>23825376902.33418</v>
+        <v>23813331260.59324</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>19264618</v>
@@ -506,13 +506,13 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>1561.3</v>
+        <v>1560.73</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>191061852691.5655</v>
+        <v>190992789187.8394</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>8044192256.696914</v>
+        <v>8048775248.455356</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>122373866.2178</v>
@@ -521,267 +521,541 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>$BNB</t>
+          <t>$USDT</t>
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>298.72</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>47784119030.06439</v>
+        <v>66490594505.92384</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>565128845.0909404</v>
+        <v>32377041275.90711</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>159979963.5904293</v>
+        <v>73141766321.23428</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>$USDT</t>
+          <t>$BNB</t>
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>1</v>
+        <v>298.83</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>66492309176.52158</v>
+        <v>47801065445.75539</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>31920124362.98594</v>
+        <v>563691854.0179112</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>73141766321.23428</v>
+        <v>159979963.5904293</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>$XRP</t>
+          <t>$USDC</t>
         </is>
       </c>
       <c r="B6" s="3" t="n">
-        <v>0.39</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>19641802424.17704</v>
+        <v>43835901598.5809</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>1250439467.963048</v>
+        <v>2901189759.720745</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>99989156648</v>
+        <v>43841459704.57129</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>$ADA</t>
+          <t>$XRP</t>
         </is>
       </c>
       <c r="B7" s="3" t="n">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>12030858722.25394</v>
+        <v>19666967859.20561</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>343670535.7675748</v>
+        <v>1227605238.703969</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>35303937971.934</v>
+        <v>99989156648</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>$ORAI</t>
+          <t>$BUSD</t>
         </is>
       </c>
       <c r="B8" s="3" t="n">
-        <v>4.36</v>
+        <v>1</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>8905604.101792807</v>
+        <v>16247560099.42515</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>1141549.20720633</v>
+        <v>8225416843.490399</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>19779272</v>
+        <v>16242596010.61406</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>$MATIC</t>
+          <t>$ADA</t>
         </is>
       </c>
       <c r="B9" s="3" t="n">
-        <v>1.01</v>
+        <v>0.35</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>8807411423.929722</v>
+        <v>12057715982.64891</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>561244644.2349737</v>
+        <v>343469550.7680789</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>10000000000</v>
+        <v>35303937971.934</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>$DOT</t>
+          <t>$DOGE</t>
         </is>
       </c>
       <c r="B10" s="3" t="n">
-        <v>5.9</v>
+        <v>0.08</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>6815578788.230002</v>
+        <v>11130913882.48604</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>278884351.3055308</v>
+        <v>461106665.3322925</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>1271962399.3702</v>
+        <v>132670764299.8941</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>$AVAX</t>
+          <t>$MATIC</t>
         </is>
       </c>
       <c r="B11" s="3" t="n">
-        <v>16.79</v>
+        <v>1.01</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>5232580697.842166</v>
+        <v>8835122977.265144</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>410554032.2522914</v>
+        <v>607386215.487919</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>416988132.7412243</v>
+        <v>10000000000</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>$TRX</t>
+          <t>$SOL</t>
         </is>
       </c>
       <c r="B12" s="3" t="n">
-        <v>0.06</v>
+        <v>23.36</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>5687845535.820404</v>
+        <v>8661677693.50992</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>229191968.0160865</v>
+        <v>1261440340.750323</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>91874796149.61217</v>
+        <v>538755344.6046014</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>$UNI</t>
+          <t>$DOT</t>
         </is>
       </c>
       <c r="B13" s="3" t="n">
-        <v>6.54</v>
+        <v>6</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>4988257663.325697</v>
+        <v>6934936947.359878</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>108562056.2261184</v>
+        <v>308301009.1270776</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>1000000000</v>
+        <v>1271962399.3702</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>$ATOM</t>
+          <t>$LTC</t>
         </is>
       </c>
       <c r="B14" s="3" t="n">
-        <v>12.5</v>
+        <v>85.7</v>
       </c>
       <c r="C14" s="3" t="n">
-        <v>3579395655.654541</v>
+        <v>6176940690.369475</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>201484103.0828425</v>
+        <v>596893939.7728382</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>0</v>
+        <v>84000000</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>$LINK</t>
+          <t>$DAI</t>
         </is>
       </c>
       <c r="B15" s="3" t="n">
-        <v>6.68</v>
+        <v>1</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>3394851143.953818</v>
+        <v>5833569481.472278</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>353138958.3440628</v>
+        <v>179521199.5863547</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>1000000000</v>
+        <v>5835995685.216533</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>$ANKR</t>
+          <t>$SHIB</t>
         </is>
       </c>
       <c r="B16" s="3" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>225266858.6251447</v>
+        <v>5754003682.647244</v>
       </c>
       <c r="D16" s="3" t="n">
-        <v>49221551.20942393</v>
+        <v>311403153.8771881</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>10000000000</v>
+        <v>589735030408322.8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>$FTM</t>
+          <t>$TRX</t>
         </is>
       </c>
       <c r="B17" s="3" t="n">
-        <v>0.32</v>
+        <v>0.06</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>887863049.509101</v>
+        <v>5700945370.103837</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>182085506.1988394</v>
+        <v>228364886.564765</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>3175000000</v>
+        <v>91874796149.61217</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>$AVAX</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="n">
+        <v>16.79</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>5230115101.594823</v>
+      </c>
+      <c r="D18" s="3" t="n">
+        <v>450337835.0047283</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>416988132.7412243</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>$UNI</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="n">
+        <v>6.55</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>4989400929.190395</v>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>107955481.4764907</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>$WBTC</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="n">
+        <v>21062.28</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>3865929525.85234</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <v>110113201.8696926</v>
+      </c>
+      <c r="E20" s="3" t="n">
+        <v>183547.54135694</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>$ATOM</t>
+        </is>
+      </c>
+      <c r="B21" s="3" t="n">
+        <v>12.45</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>3565281172.250839</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <v>201600933.9508532</v>
+      </c>
+      <c r="E21" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>$LINK</t>
+        </is>
+      </c>
+      <c r="B22" s="3" t="n">
+        <v>6.71</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>3406832494.598842</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <v>358928028.7217537</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>$LEO</t>
+        </is>
+      </c>
+      <c r="B23" s="3" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>3314007895.554636</v>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>2358953.69817772</v>
+      </c>
+      <c r="E23" s="3" t="n">
+        <v>985239504</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>$XMR</t>
+        </is>
+      </c>
+      <c r="B24" s="3" t="n">
+        <v>171.25</v>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>3121561109.13796</v>
+      </c>
+      <c r="D24" s="3" t="n">
+        <v>93090638.92516409</v>
+      </c>
+      <c r="E24" s="3" t="n">
+        <v>18228028.59174703</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>$ETC</t>
+        </is>
+      </c>
+      <c r="B25" s="3" t="n">
+        <v>22.35</v>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>3104496982.653294</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>244667031.6846894</v>
+      </c>
+      <c r="E25" s="3" t="n">
+        <v>210700000</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>$TON</t>
+        </is>
+      </c>
+      <c r="B26" s="3" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>2837885231.549485</v>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>33460868.23835777</v>
+      </c>
+      <c r="E26" s="3" t="n">
+        <v>5047558528</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>$BCH</t>
+        </is>
+      </c>
+      <c r="B27" s="3" t="n">
+        <v>124.77</v>
+      </c>
+      <c r="C27" s="3" t="n">
+        <v>2406407891.330467</v>
+      </c>
+      <c r="D27" s="3" t="n">
+        <v>219252338.7187677</v>
+      </c>
+      <c r="E27" s="3" t="n">
+        <v>19286118.75</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>$XLM</t>
+        </is>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="C28" s="3" t="n">
+        <v>2265896764.437149</v>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>63037359.2597696</v>
+      </c>
+      <c r="E28" s="3" t="n">
+        <v>50001787494.60719</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>$CRO</t>
+        </is>
+      </c>
+      <c r="B29" s="3" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="C29" s="3" t="n">
+        <v>1992142691.202807</v>
+      </c>
+      <c r="D29" s="3" t="n">
+        <v>88615368.63830242</v>
+      </c>
+      <c r="E29" s="3" t="n">
+        <v>30263013692</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>$OKB</t>
+        </is>
+      </c>
+      <c r="B30" s="3" t="n">
+        <v>31.44</v>
+      </c>
+      <c r="C30" s="3" t="n">
+        <v>1886453324.786516</v>
+      </c>
+      <c r="D30" s="3" t="n">
+        <v>22055353.68384389</v>
+      </c>
+      <c r="E30" s="3" t="n">
+        <v>300000000</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>$NEAR</t>
+        </is>
+      </c>
+      <c r="B31" s="3" t="inlineStr">
+        <is>
+          <t>Erreur</t>
+        </is>
+      </c>
+      <c r="C31" s="3" t="inlineStr">
+        <is>
+          <t>Erreur</t>
+        </is>
+      </c>
+      <c r="D31" s="3" t="inlineStr">
+        <is>
+          <t>Erreur</t>
+        </is>
+      </c>
+      <c r="E31" s="3" t="inlineStr">
+        <is>
+          <t>Erreur</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add CMC rank + fix font issues
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -26,13 +26,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <b val="1"/>
+      <sz val="14"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <color rgb="00FFFFFF"/>
-    </font>
-    <font>
       <sz val="14"/>
     </font>
   </fonts>
@@ -70,9 +68,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -438,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,10 +445,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="9.6" customWidth="1" min="1" max="1"/>
-    <col width="9.6" customWidth="1" min="2" max="2"/>
+    <col width="7.199999999999999" customWidth="1" min="2" max="2"/>
     <col width="13.2" customWidth="1" min="3" max="3"/>
     <col width="20.4" customWidth="1" min="4" max="4"/>
     <col width="16.8" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -479,6 +478,11 @@
           <t>TOTAL SUPPLY</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>RANG CMC</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -487,16 +491,19 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>21084.02</v>
+        <v>21168.83</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>406175601662.3179</v>
+        <v>407811455280.153</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>23813331260.59324</v>
+        <v>22339245370.33652</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>19264618</v>
+        <v>19264718</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -506,17 +513,20 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>1560.73</v>
+        <v>1565.64</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>190992789187.8394</v>
+        <v>191593350364.9316</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>8048775248.455356</v>
+        <v>7448431970.075871</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>122373866.2178</v>
       </c>
+      <c r="F3" s="3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
@@ -528,14 +538,17 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>66490594505.92384</v>
+        <v>66491107167.65922</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>32377041275.90711</v>
+        <v>30214762894.26654</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>73141766321.23428</v>
       </c>
+      <c r="F4" s="3" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
@@ -544,17 +557,20 @@
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>298.83</v>
+        <v>301.36</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>47801065445.75539</v>
+        <v>47585582469.44303</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>563691854.0179112</v>
+        <v>538105890.2211037</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>159979963.5904293</v>
       </c>
+      <c r="F5" s="3" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
@@ -566,13 +582,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>43835901598.5809</v>
+        <v>43862353349.50217</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>2901189759.720745</v>
+        <v>2808076162.088495</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>43841459704.57129</v>
+        <v>43864338104.48129</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -585,14 +604,17 @@
         <v>0.39</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>19666967859.20561</v>
+        <v>19688994638.56188</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>1227605238.703969</v>
+        <v>1066705439.564966</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>99989156648</v>
       </c>
+      <c r="F7" s="3" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
@@ -604,14 +626,17 @@
         <v>1</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>16247560099.42515</v>
+        <v>16247411747.80642</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>8225416843.490399</v>
+        <v>7744563187.072851</v>
       </c>
       <c r="E8" s="3" t="n">
         <v>16242596010.61406</v>
       </c>
+      <c r="F8" s="3" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
@@ -623,14 +648,17 @@
         <v>0.35</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>12057715982.64891</v>
+        <v>12110045788.8835</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>343469550.7680789</v>
+        <v>305659364.4982858</v>
       </c>
       <c r="E9" s="3" t="n">
         <v>35303937971.934</v>
       </c>
+      <c r="F9" s="3" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
@@ -642,14 +670,17 @@
         <v>0.08</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>11130913882.48604</v>
+        <v>11158541628.06409</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>461106665.3322925</v>
+        <v>410925814.8691707</v>
       </c>
       <c r="E10" s="3" t="n">
         <v>132670764299.8941</v>
       </c>
+      <c r="F10" s="3" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
@@ -661,14 +692,17 @@
         <v>1.01</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>8835122977.265144</v>
+        <v>8843320015.515112</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>607386215.487919</v>
+        <v>538079421.8554176</v>
       </c>
       <c r="E11" s="3" t="n">
         <v>10000000000</v>
       </c>
+      <c r="F11" s="3" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
@@ -677,16 +711,19 @@
         </is>
       </c>
       <c r="B12" s="3" t="n">
-        <v>23.36</v>
+        <v>23.52</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>8661677693.50992</v>
+        <v>8720554480.201212</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>1261440340.750323</v>
+        <v>1094501924.404907</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>538755344.6046014</v>
+        <v>538755267.1040359</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="13">
@@ -696,16 +733,19 @@
         </is>
       </c>
       <c r="B13" s="3" t="n">
-        <v>6</v>
+        <v>5.99</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>6934936947.359878</v>
+        <v>6926838126.564939</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>308301009.1270776</v>
+        <v>283493632.5928709</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>1271962399.3702</v>
+        <v>1271963851.44491</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="14">
@@ -715,17 +755,20 @@
         </is>
       </c>
       <c r="B14" s="3" t="n">
-        <v>85.7</v>
+        <v>85.92</v>
       </c>
       <c r="C14" s="3" t="n">
-        <v>6176940690.369475</v>
+        <v>6192701772.203585</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>596893939.7728382</v>
+        <v>529802885.1792039</v>
       </c>
       <c r="E14" s="3" t="n">
         <v>84000000</v>
       </c>
+      <c r="F14" s="3" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
@@ -737,13 +780,16 @@
         <v>1</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>5833569481.472278</v>
+        <v>5834209597.046004</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>179521199.5863547</v>
+        <v>176350768.4856356</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>5835995685.216533</v>
+        <v>5836021298.701854</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="16">
@@ -756,14 +802,17 @@
         <v>0</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>5754003682.647244</v>
+        <v>5763941815.889625</v>
       </c>
       <c r="D16" s="3" t="n">
-        <v>311403153.8771881</v>
+        <v>283271667.7532188</v>
       </c>
       <c r="E16" s="3" t="n">
         <v>589735030408322.8</v>
       </c>
+      <c r="F16" s="3" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
@@ -775,13 +824,16 @@
         <v>0.06</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>5700945370.103837</v>
+        <v>5724157373.978841</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>228364886.564765</v>
+        <v>212359066.5579945</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>91874796149.61217</v>
+        <v>91873986399.15848</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="18">
@@ -791,17 +843,20 @@
         </is>
       </c>
       <c r="B18" s="3" t="n">
-        <v>16.79</v>
+        <v>16.88</v>
       </c>
       <c r="C18" s="3" t="n">
-        <v>5230115101.594823</v>
+        <v>5261026258.208487</v>
       </c>
       <c r="D18" s="3" t="n">
-        <v>450337835.0047283</v>
+        <v>405552238.1652377</v>
       </c>
       <c r="E18" s="3" t="n">
         <v>416988132.7412243</v>
       </c>
+      <c r="F18" s="3" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
@@ -810,17 +865,20 @@
         </is>
       </c>
       <c r="B19" s="3" t="n">
-        <v>6.55</v>
+        <v>6.56</v>
       </c>
       <c r="C19" s="3" t="n">
-        <v>4989400929.190395</v>
+        <v>4996484421.736659</v>
       </c>
       <c r="D19" s="3" t="n">
-        <v>107955481.4764907</v>
+        <v>97314359.43741956</v>
       </c>
       <c r="E19" s="3" t="n">
         <v>1000000000</v>
       </c>
+      <c r="F19" s="3" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
@@ -829,17 +887,20 @@
         </is>
       </c>
       <c r="B20" s="3" t="n">
-        <v>21062.28</v>
+        <v>21140.39</v>
       </c>
       <c r="C20" s="3" t="n">
-        <v>3865929525.85234</v>
+        <v>3880267348.112655</v>
       </c>
       <c r="D20" s="3" t="n">
-        <v>110113201.8696926</v>
+        <v>99970112.21350345</v>
       </c>
       <c r="E20" s="3" t="n">
         <v>183547.54135694</v>
       </c>
+      <c r="F20" s="3" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
@@ -848,17 +909,20 @@
         </is>
       </c>
       <c r="B21" s="3" t="n">
-        <v>12.45</v>
+        <v>12.58</v>
       </c>
       <c r="C21" s="3" t="n">
-        <v>3565281172.250839</v>
+        <v>3603376088.400484</v>
       </c>
       <c r="D21" s="3" t="n">
-        <v>201600933.9508532</v>
+        <v>191819146.8054051</v>
       </c>
       <c r="E21" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="F21" s="3" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
@@ -870,14 +934,17 @@
         <v>6.71</v>
       </c>
       <c r="C22" s="3" t="n">
-        <v>3406832494.598842</v>
+        <v>3407697751.628366</v>
       </c>
       <c r="D22" s="3" t="n">
-        <v>358928028.7217537</v>
+        <v>325533488.5516467</v>
       </c>
       <c r="E22" s="3" t="n">
         <v>1000000000</v>
       </c>
+      <c r="F22" s="3" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
@@ -889,14 +956,17 @@
         <v>3.47</v>
       </c>
       <c r="C23" s="3" t="n">
-        <v>3314007895.554636</v>
+        <v>3313806734.846179</v>
       </c>
       <c r="D23" s="3" t="n">
-        <v>2358953.69817772</v>
+        <v>2223711.1581114</v>
       </c>
       <c r="E23" s="3" t="n">
         <v>985239504</v>
       </c>
+      <c r="F23" s="3" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
@@ -905,16 +975,19 @@
         </is>
       </c>
       <c r="B24" s="3" t="n">
-        <v>171.25</v>
+        <v>171.69</v>
       </c>
       <c r="C24" s="3" t="n">
-        <v>3121561109.13796</v>
+        <v>3129545885.786795</v>
       </c>
       <c r="D24" s="3" t="n">
-        <v>93090638.92516409</v>
+        <v>81592756.11596856</v>
       </c>
       <c r="E24" s="3" t="n">
-        <v>18228028.59174703</v>
+        <v>18228070.59174703</v>
+      </c>
+      <c r="F24" s="3" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="25">
@@ -924,17 +997,20 @@
         </is>
       </c>
       <c r="B25" s="3" t="n">
-        <v>22.35</v>
+        <v>22.28</v>
       </c>
       <c r="C25" s="3" t="n">
-        <v>3104496982.653294</v>
+        <v>3094995853.677303</v>
       </c>
       <c r="D25" s="3" t="n">
-        <v>244667031.6846894</v>
+        <v>222566641.0576102</v>
       </c>
       <c r="E25" s="3" t="n">
         <v>210700000</v>
       </c>
+      <c r="F25" s="3" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
@@ -943,17 +1019,20 @@
         </is>
       </c>
       <c r="B26" s="3" t="n">
-        <v>2.32</v>
+        <v>2.33</v>
       </c>
       <c r="C26" s="3" t="n">
-        <v>2837885231.549485</v>
+        <v>2843573657.019699</v>
       </c>
       <c r="D26" s="3" t="n">
-        <v>33460868.23835777</v>
+        <v>32978319.8624108</v>
       </c>
       <c r="E26" s="3" t="n">
         <v>5047558528</v>
       </c>
+      <c r="F26" s="3" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="inlineStr">
@@ -962,16 +1041,19 @@
         </is>
       </c>
       <c r="B27" s="3" t="n">
-        <v>124.77</v>
+        <v>124.61</v>
       </c>
       <c r="C27" s="3" t="n">
-        <v>2406407891.330467</v>
+        <v>2403288579.758314</v>
       </c>
       <c r="D27" s="3" t="n">
-        <v>219252338.7187677</v>
+        <v>207787414.3643877</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>19286118.75</v>
+        <v>19286206.25</v>
+      </c>
+      <c r="F27" s="3" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="28">
@@ -984,14 +1066,17 @@
         <v>0.09</v>
       </c>
       <c r="C28" s="3" t="n">
-        <v>2265896764.437149</v>
+        <v>2275392116.639856</v>
       </c>
       <c r="D28" s="3" t="n">
-        <v>63037359.2597696</v>
+        <v>55911154.57314705</v>
       </c>
       <c r="E28" s="3" t="n">
         <v>50001787494.60719</v>
       </c>
+      <c r="F28" s="3" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
@@ -1003,59 +1088,38 @@
         <v>0.08</v>
       </c>
       <c r="C29" s="3" t="n">
-        <v>1992142691.202807</v>
+        <v>1992708945.661148</v>
       </c>
       <c r="D29" s="3" t="n">
-        <v>88615368.63830242</v>
+        <v>60230378.54025527</v>
       </c>
       <c r="E29" s="3" t="n">
         <v>30263013692</v>
       </c>
+      <c r="F29" s="3" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
-          <t>$OKB</t>
+          <t>$NEAR</t>
         </is>
       </c>
       <c r="B30" s="3" t="n">
-        <v>31.44</v>
+        <v>2.23</v>
       </c>
       <c r="C30" s="3" t="n">
-        <v>1886453324.786516</v>
+        <v>1898216853.338375</v>
       </c>
       <c r="D30" s="3" t="n">
-        <v>22055353.68384389</v>
+        <v>192237322.0720434</v>
       </c>
       <c r="E30" s="3" t="n">
-        <v>300000000</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="2" t="inlineStr">
-        <is>
-          <t>$NEAR</t>
-        </is>
-      </c>
-      <c r="B31" s="3" t="inlineStr">
-        <is>
-          <t>Erreur</t>
-        </is>
-      </c>
-      <c r="C31" s="3" t="inlineStr">
-        <is>
-          <t>Erreur</t>
-        </is>
-      </c>
-      <c r="D31" s="3" t="inlineStr">
-        <is>
-          <t>Erreur</t>
-        </is>
-      </c>
-      <c r="E31" s="3" t="inlineStr">
-        <is>
-          <t>Erreur</t>
-        </is>
+        <v>1000000000</v>
+      </c>
+      <c r="F30" s="3" t="n">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>